<commit_message>
modified payment receipt form
</commit_message>
<xml_diff>
--- a/files/Authorize.xlsx
+++ b/files/Authorize.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITAdmin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ehsan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C9E294-40D3-44C9-8D23-AEED1E05719D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FA949F-F785-4B22-8615-ED5BF7F6A3EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11865" xr2:uid="{EAFF9FC7-1C66-4BDC-88CA-566F655ADB0F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EAFF9FC7-1C66-4BDC-88CA-566F655ADB0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="273">
   <si>
     <t>Response Code</t>
   </si>
@@ -194,12 +194,6 @@
     <t>AUTH_CAPTURE</t>
   </si>
   <si>
-    <t>Emilio</t>
-  </si>
-  <si>
-    <t>Achar</t>
-  </si>
-  <si>
     <t>Eucaliptp 22 601 CD</t>
   </si>
   <si>
@@ -245,12 +239,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>MARIO EDGARDO</t>
-  </si>
-  <si>
-    <t>FONSECA LAINEZ</t>
-  </si>
-  <si>
     <t>Colonia Bantral, 2da calle, a mano izquierda.</t>
   </si>
   <si>
@@ -272,9 +260,6 @@
     <t>rolando alberto sabillon calix 33636062 1MU17-25392</t>
   </si>
   <si>
-    <t>lourdes</t>
-  </si>
-  <si>
     <t>marquez</t>
   </si>
   <si>
@@ -299,9 +284,6 @@
     <t>Joseph Frantz Leonard 50937292068 1MU18-26212</t>
   </si>
   <si>
-    <t>Josepg Frantz</t>
-  </si>
-  <si>
     <t>Leonard</t>
   </si>
   <si>
@@ -332,9 +314,6 @@
     <t>Mario</t>
   </si>
   <si>
-    <t>Boquin</t>
-  </si>
-  <si>
     <t>Col. Lomas del guijarro sur calle paris casa 3801</t>
   </si>
   <si>
@@ -356,9 +335,6 @@
     <t>CREDIT</t>
   </si>
   <si>
-    <t>Justo</t>
-  </si>
-  <si>
     <t>Crespo</t>
   </si>
   <si>
@@ -572,9 +548,6 @@
     <t>JORG ZINECKER 593998121459 1MU18-26007</t>
   </si>
   <si>
-    <t>MARIA NELSY</t>
-  </si>
-  <si>
     <t>RODRIGUEZ</t>
   </si>
   <si>
@@ -827,9 +800,6 @@
     <t>isaac</t>
   </si>
   <si>
-    <t>alfille</t>
-  </si>
-  <si>
     <t>hacienda del ciervo 28</t>
   </si>
   <si>
@@ -840,6 +810,45 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Achar'</t>
+  </si>
+  <si>
+    <t>Boquin"'</t>
+  </si>
+  <si>
+    <t>FONSECA LAINEZ'</t>
+  </si>
+  <si>
+    <t>alfille"'"</t>
+  </si>
+  <si>
+    <t>GENCON"'"'</t>
+  </si>
+  <si>
+    <t>MARIO EDGARDO'</t>
+  </si>
+  <si>
+    <t>lourdes'</t>
+  </si>
+  <si>
+    <t>Josepg Frantz'</t>
+  </si>
+  <si>
+    <t>Emilio'</t>
+  </si>
+  <si>
+    <t>Justo'"/'</t>
+  </si>
+  <si>
+    <t>JOSE'</t>
+  </si>
+  <si>
+    <t>MARIA NELSY'</t>
+  </si>
+  <si>
+    <t>ANDRES'</t>
   </si>
 </sst>
 </file>
@@ -1194,14 +1203,18 @@
   <dimension ref="A1:AV30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A30"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="23.5703125" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1386,46 +1399,46 @@
         <v>53</v>
       </c>
       <c r="O2" t="s">
+        <v>268</v>
+      </c>
+      <c r="P2" t="s">
+        <v>260</v>
+      </c>
+      <c r="R2" t="s">
         <v>54</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>55</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>56</v>
-      </c>
-      <c r="S2" t="s">
-        <v>57</v>
-      </c>
-      <c r="T2" t="s">
-        <v>58</v>
       </c>
       <c r="U2">
         <v>52785</v>
       </c>
       <c r="V2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="W2">
         <v>15530387727</v>
       </c>
       <c r="Y2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP2" t="s">
         <v>60</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AQ2" t="s">
         <v>61</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AU2" t="s">
         <v>62</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AV2" t="s">
         <v>63</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
@@ -1439,16 +1452,16 @@
         <v>471246</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3">
         <v>41016455705</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H3" t="s">
         <v>50</v>
@@ -1457,52 +1470,52 @@
         <v>20181025034235</v>
       </c>
       <c r="J3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K3">
         <v>329</v>
       </c>
       <c r="L3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M3" t="s">
         <v>53</v>
       </c>
       <c r="O3" t="s">
+        <v>265</v>
+      </c>
+      <c r="P3" t="s">
+        <v>262</v>
+      </c>
+      <c r="R3" t="s">
+        <v>69</v>
+      </c>
+      <c r="S3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3" t="s">
         <v>71</v>
-      </c>
-      <c r="P3" t="s">
-        <v>72</v>
-      </c>
-      <c r="R3" t="s">
-        <v>73</v>
-      </c>
-      <c r="S3" t="s">
-        <v>74</v>
-      </c>
-      <c r="V3" t="s">
-        <v>75</v>
       </c>
       <c r="W3">
         <v>50431892375</v>
       </c>
       <c r="Y3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="AK3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ3" t="s">
         <v>61</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AU3" t="s">
         <v>62</v>
       </c>
-      <c r="AQ3" t="s">
+      <c r="AV3" t="s">
         <v>63</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
@@ -1516,16 +1529,16 @@
         <v>536696</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E4">
         <v>41016801107</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
         <v>50</v>
@@ -1534,52 +1547,52 @@
         <v>20181025094558</v>
       </c>
       <c r="J4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K4">
         <v>107.6</v>
       </c>
       <c r="L4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M4" t="s">
         <v>53</v>
       </c>
       <c r="O4" t="s">
-        <v>80</v>
+        <v>266</v>
       </c>
       <c r="P4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="R4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="S4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="V4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="W4">
         <v>33636062</v>
       </c>
       <c r="Y4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="AK4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ4" t="s">
         <v>61</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AU4" t="s">
         <v>62</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AV4" t="s">
         <v>63</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
@@ -1593,16 +1606,16 @@
         <v>2041</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E5">
         <v>41016841907</v>
       </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s">
         <v>50</v>
@@ -1611,52 +1624,52 @@
         <v>20181025100817</v>
       </c>
       <c r="J5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="K5">
         <v>462</v>
       </c>
       <c r="L5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M5" t="s">
         <v>53</v>
       </c>
       <c r="O5" t="s">
+        <v>267</v>
+      </c>
+      <c r="P5" t="s">
+        <v>84</v>
+      </c>
+      <c r="R5" t="s">
+        <v>85</v>
+      </c>
+      <c r="S5" t="s">
+        <v>86</v>
+      </c>
+      <c r="U5" t="s">
+        <v>87</v>
+      </c>
+      <c r="V5" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y5" t="s">
         <v>89</v>
       </c>
-      <c r="P5" t="s">
-        <v>90</v>
-      </c>
-      <c r="R5" t="s">
-        <v>91</v>
-      </c>
-      <c r="S5" t="s">
-        <v>92</v>
-      </c>
-      <c r="U5" t="s">
-        <v>93</v>
-      </c>
-      <c r="V5" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>95</v>
-      </c>
       <c r="AK5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ5" t="s">
         <v>61</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AU5" t="s">
         <v>62</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="AV5" t="s">
         <v>63</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.25">
@@ -1670,16 +1683,16 @@
         <v>6177</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E6">
         <v>41016847116</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H6" t="s">
         <v>50</v>
@@ -1688,52 +1701,52 @@
         <v>20181025100757</v>
       </c>
       <c r="J6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="K6">
         <v>730</v>
       </c>
       <c r="L6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M6" t="s">
         <v>53</v>
       </c>
       <c r="O6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="P6" t="s">
-        <v>100</v>
+        <v>261</v>
       </c>
       <c r="R6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="S6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="V6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="W6">
         <v>98799045</v>
       </c>
       <c r="Y6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="AK6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ6" t="s">
         <v>61</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AU6" t="s">
         <v>62</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AV6" t="s">
         <v>63</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
@@ -1744,16 +1757,16 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E7">
         <v>61356138009</v>
       </c>
       <c r="F7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G7" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="H7" t="s">
         <v>50</v>
@@ -1762,49 +1775,49 @@
         <v>20181017120516</v>
       </c>
       <c r="J7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="K7">
         <v>150</v>
       </c>
       <c r="L7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>108</v>
+        <v>269</v>
       </c>
       <c r="P7" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="R7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="S7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="V7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Y7" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="AK7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ7" t="s">
         <v>61</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AU7" t="s">
         <v>62</v>
       </c>
-      <c r="AQ7" t="s">
+      <c r="AV7" t="s">
         <v>63</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
@@ -1818,16 +1831,16 @@
         <v>6980</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E8">
         <v>41017030326</v>
       </c>
       <c r="F8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H8" t="s">
         <v>50</v>
@@ -1836,52 +1849,52 @@
         <v>20181025115319</v>
       </c>
       <c r="J8" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="K8">
         <v>365</v>
       </c>
       <c r="L8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M8" t="s">
         <v>53</v>
       </c>
       <c r="O8" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="P8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="R8" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="S8" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="V8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="W8">
         <v>50431892375</v>
       </c>
       <c r="Y8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="AK8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ8" t="s">
         <v>61</v>
       </c>
-      <c r="AP8" t="s">
+      <c r="AU8" t="s">
         <v>62</v>
       </c>
-      <c r="AQ8" t="s">
+      <c r="AV8" t="s">
         <v>63</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
@@ -1895,16 +1908,16 @@
         <v>1494</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E9">
         <v>41017337670</v>
       </c>
       <c r="F9" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G9" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H9" t="s">
         <v>50</v>
@@ -1913,52 +1926,52 @@
         <v>20181025144856</v>
       </c>
       <c r="J9" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="K9">
         <v>1241.9000000000001</v>
       </c>
       <c r="L9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M9" t="s">
         <v>53</v>
       </c>
       <c r="O9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="P9" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="R9" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="S9" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="V9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="W9">
         <v>8095663673</v>
       </c>
       <c r="Y9" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="AK9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ9" t="s">
         <v>61</v>
       </c>
-      <c r="AP9" t="s">
+      <c r="AU9" t="s">
         <v>62</v>
       </c>
-      <c r="AQ9" t="s">
+      <c r="AV9" t="s">
         <v>63</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
@@ -1972,16 +1985,16 @@
         <v>135929</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E10">
         <v>41017486586</v>
       </c>
       <c r="F10" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="G10" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H10" t="s">
         <v>50</v>
@@ -1990,7 +2003,7 @@
         <v>20181025161748</v>
       </c>
       <c r="J10" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="K10">
         <v>1140.3</v>
@@ -2002,40 +2015,40 @@
         <v>53</v>
       </c>
       <c r="O10" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="P10" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="R10" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="S10" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="V10" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="W10" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="Y10" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="AK10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ10" t="s">
         <v>61</v>
       </c>
-      <c r="AP10" t="s">
+      <c r="AU10" t="s">
         <v>62</v>
       </c>
-      <c r="AQ10" t="s">
+      <c r="AV10" t="s">
         <v>63</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV10" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -2049,16 +2062,16 @@
         <v>25989</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E11">
         <v>41017563887</v>
       </c>
       <c r="F11" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G11" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H11" t="s">
         <v>50</v>
@@ -2067,49 +2080,49 @@
         <v>20181025172330</v>
       </c>
       <c r="J11" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="K11">
         <v>456.5</v>
       </c>
       <c r="L11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M11" t="s">
         <v>53</v>
       </c>
       <c r="O11" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="P11" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="R11" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="S11" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="V11" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="Y11" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="AK11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ11" t="s">
         <v>61</v>
       </c>
-      <c r="AP11" t="s">
+      <c r="AU11" t="s">
         <v>62</v>
       </c>
-      <c r="AQ11" t="s">
+      <c r="AV11" t="s">
         <v>63</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV11" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.25">
@@ -2120,16 +2133,16 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E12">
         <v>41017642844</v>
       </c>
       <c r="F12" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G12" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H12" t="s">
         <v>50</v>
@@ -2138,49 +2151,49 @@
         <v>20181025183125</v>
       </c>
       <c r="J12" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="K12">
         <v>2286</v>
       </c>
       <c r="L12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M12" t="s">
         <v>53</v>
       </c>
       <c r="O12" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="P12" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="R12" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S12" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="V12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="Y12" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="AK12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU12" t="s">
         <v>62</v>
       </c>
-      <c r="AQ12" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU12" t="s">
-        <v>64</v>
-      </c>
       <c r="AV12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.25">
@@ -2191,19 +2204,19 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D13" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E13">
         <v>41017846447</v>
       </c>
       <c r="F13" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G13" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H13" t="s">
         <v>50</v>
@@ -2212,61 +2225,61 @@
         <v>20181025221325</v>
       </c>
       <c r="J13" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="K13">
         <v>282.5</v>
       </c>
       <c r="L13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M13" t="s">
         <v>53</v>
       </c>
       <c r="O13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="P13" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="R13" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="S13" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="T13" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="U13">
         <v>60202</v>
       </c>
       <c r="V13" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="W13">
         <v>99456170</v>
       </c>
       <c r="X13" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="Y13" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="AK13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU13" t="s">
         <v>62</v>
       </c>
-      <c r="AQ13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>64</v>
-      </c>
       <c r="AV13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.25">
@@ -2280,16 +2293,16 @@
         <v>886331</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E14">
         <v>41018441863</v>
       </c>
       <c r="F14" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="G14" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="H14" t="s">
         <v>50</v>
@@ -2298,52 +2311,52 @@
         <v>20181026085437</v>
       </c>
       <c r="J14" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="K14">
         <v>181.45</v>
       </c>
       <c r="L14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M14" t="s">
         <v>53</v>
       </c>
       <c r="O14" t="s">
-        <v>168</v>
+        <v>270</v>
       </c>
       <c r="P14" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="R14" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="S14" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="T14" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="V14" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="Y14" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="AK14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU14" t="s">
         <v>62</v>
       </c>
-      <c r="AQ14" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>64</v>
-      </c>
       <c r="AV14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.25">
@@ -2357,16 +2370,16 @@
         <v>886560</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E15">
         <v>41018455607</v>
       </c>
       <c r="F15" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="G15" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="H15" t="s">
         <v>50</v>
@@ -2375,52 +2388,52 @@
         <v>20181026090133</v>
       </c>
       <c r="J15" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="K15">
         <v>83.3</v>
       </c>
       <c r="L15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M15" t="s">
         <v>53</v>
       </c>
       <c r="O15" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="P15" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="R15" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="S15" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="T15" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="V15" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="Y15" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="AK15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU15" t="s">
         <v>62</v>
       </c>
-      <c r="AQ15" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU15" t="s">
-        <v>64</v>
-      </c>
       <c r="AV15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.25">
@@ -2434,16 +2447,16 @@
         <v>343328</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E16">
         <v>41018725486</v>
       </c>
       <c r="F16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="G16" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="H16" t="s">
         <v>50</v>
@@ -2452,7 +2465,7 @@
         <v>20181026111547</v>
       </c>
       <c r="J16" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="K16">
         <v>430.2</v>
@@ -2464,37 +2477,37 @@
         <v>53</v>
       </c>
       <c r="O16" t="s">
-        <v>180</v>
+        <v>271</v>
       </c>
       <c r="P16" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="R16" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="S16" t="s">
+        <v>135</v>
+      </c>
+      <c r="V16" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ16" t="s">
         <v>143</v>
       </c>
-      <c r="V16" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>145</v>
-      </c>
-      <c r="AK16" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP16" t="s">
+      <c r="AU16" t="s">
         <v>62</v>
       </c>
-      <c r="AQ16" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU16" t="s">
-        <v>64</v>
-      </c>
       <c r="AV16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.25">
@@ -2508,16 +2521,16 @@
         <v>555365</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E17">
         <v>41018783977</v>
       </c>
       <c r="F17" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G17" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="H17" t="s">
         <v>50</v>
@@ -2526,55 +2539,55 @@
         <v>20181026114424</v>
       </c>
       <c r="J17" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="K17">
         <v>109.84</v>
       </c>
       <c r="L17" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="M17" t="s">
         <v>53</v>
       </c>
       <c r="O17" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="P17" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="R17" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="S17" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="T17" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="V17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="W17">
         <v>31892375</v>
       </c>
       <c r="Y17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="AK17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU17" t="s">
         <v>62</v>
       </c>
-      <c r="AQ17" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU17" t="s">
-        <v>64</v>
-      </c>
       <c r="AV17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.25">
@@ -2588,16 +2601,16 @@
         <v>11666</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E18">
         <v>41018851544</v>
       </c>
       <c r="F18" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G18" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H18" t="s">
         <v>50</v>
@@ -2606,49 +2619,49 @@
         <v>20181026122029</v>
       </c>
       <c r="J18" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="K18">
         <v>200.7</v>
       </c>
       <c r="L18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M18" t="s">
         <v>53</v>
       </c>
       <c r="O18" t="s">
-        <v>140</v>
+        <v>272</v>
       </c>
       <c r="P18" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="R18" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="S18" t="s">
+        <v>135</v>
+      </c>
+      <c r="V18" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ18" t="s">
         <v>143</v>
       </c>
-      <c r="V18" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>145</v>
-      </c>
-      <c r="AK18" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP18" t="s">
+      <c r="AU18" t="s">
         <v>62</v>
       </c>
-      <c r="AQ18" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU18" t="s">
-        <v>64</v>
-      </c>
       <c r="AV18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.25">
@@ -2662,16 +2675,16 @@
         <v>651864</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E19">
         <v>41019396276</v>
       </c>
       <c r="F19" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="G19" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="H19" t="s">
         <v>50</v>
@@ -2680,55 +2693,55 @@
         <v>20181026173635</v>
       </c>
       <c r="J19" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="K19">
         <v>3729</v>
       </c>
       <c r="L19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M19" t="s">
         <v>53</v>
       </c>
       <c r="O19" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="P19" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="R19" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="S19" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="T19" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="V19" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="W19">
         <v>22743477</v>
       </c>
       <c r="Y19" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="AK19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU19" t="s">
         <v>62</v>
       </c>
-      <c r="AQ19" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU19" t="s">
-        <v>64</v>
-      </c>
       <c r="AV19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.25">
@@ -2742,16 +2755,16 @@
         <v>893220</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20">
         <v>61360231850</v>
       </c>
       <c r="F20" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="G20" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="H20" t="s">
         <v>50</v>
@@ -2760,58 +2773,58 @@
         <v>20181027144408</v>
       </c>
       <c r="J20" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="K20">
         <v>136.5</v>
       </c>
       <c r="L20" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="M20" t="s">
         <v>53</v>
       </c>
       <c r="O20" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="P20" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="R20" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="S20" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="T20" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="U20">
         <v>593</v>
       </c>
       <c r="V20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="W20">
         <v>997202510</v>
       </c>
       <c r="Y20" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="AK20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP20" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ20" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU20" t="s">
         <v>62</v>
       </c>
-      <c r="AQ20" t="s">
-        <v>212</v>
-      </c>
-      <c r="AU20" t="s">
-        <v>64</v>
-      </c>
       <c r="AV20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.25">
@@ -2828,10 +2841,10 @@
         <v>61360245219</v>
       </c>
       <c r="F21" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G21" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="H21" t="s">
         <v>50</v>
@@ -2840,7 +2853,7 @@
         <v>20181027145103</v>
       </c>
       <c r="J21" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="K21">
         <v>176</v>
@@ -2852,46 +2865,46 @@
         <v>53</v>
       </c>
       <c r="O21" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="P21" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="R21" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="S21" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="T21" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="U21">
         <v>593</v>
       </c>
       <c r="V21" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="W21">
         <v>997202510</v>
       </c>
       <c r="Y21" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="AK21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU21" t="s">
         <v>62</v>
       </c>
-      <c r="AQ21" t="s">
-        <v>212</v>
-      </c>
-      <c r="AU21" t="s">
-        <v>64</v>
-      </c>
       <c r="AV21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.25">
@@ -2902,16 +2915,16 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E22">
         <v>61360255606</v>
       </c>
       <c r="F22" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G22" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H22" t="s">
         <v>50</v>
@@ -2920,58 +2933,58 @@
         <v>20181027145617</v>
       </c>
       <c r="J22" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K22">
         <v>385.8</v>
       </c>
       <c r="L22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M22" t="s">
         <v>53</v>
       </c>
       <c r="O22" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="P22" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="R22" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S22" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="T22" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="U22">
         <v>593</v>
       </c>
       <c r="V22" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="W22">
         <v>997202510</v>
       </c>
       <c r="Y22" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="AK22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU22" t="s">
         <v>62</v>
       </c>
-      <c r="AQ22" t="s">
-        <v>212</v>
-      </c>
-      <c r="AU22" t="s">
-        <v>64</v>
-      </c>
       <c r="AV22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.25">
@@ -2991,10 +3004,10 @@
         <v>61360278663</v>
       </c>
       <c r="F23" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="G23" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="H23" t="s">
         <v>50</v>
@@ -3003,7 +3016,7 @@
         <v>20181027150217</v>
       </c>
       <c r="J23" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="K23">
         <v>4079.55</v>
@@ -3015,46 +3028,46 @@
         <v>53</v>
       </c>
       <c r="O23" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="P23" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="R23" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="S23" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="T23" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="U23">
         <v>593</v>
       </c>
       <c r="V23" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="W23">
         <v>997202510</v>
       </c>
       <c r="Y23" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="AK23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP23" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU23" t="s">
         <v>62</v>
       </c>
-      <c r="AQ23" t="s">
-        <v>212</v>
-      </c>
-      <c r="AU23" t="s">
-        <v>64</v>
-      </c>
       <c r="AV23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.25">
@@ -3065,16 +3078,16 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E24">
         <v>61361735926</v>
       </c>
       <c r="F24" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="G24" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H24" t="s">
         <v>50</v>
@@ -3083,58 +3096,58 @@
         <v>20181028074610</v>
       </c>
       <c r="J24" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K24">
         <v>385.8</v>
       </c>
       <c r="L24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M24" t="s">
         <v>53</v>
       </c>
       <c r="O24" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="P24" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="R24" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="S24" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="T24" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="U24">
         <v>593</v>
       </c>
       <c r="V24" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="W24">
         <v>997202510</v>
       </c>
       <c r="Y24" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="AK24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP24" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ24" t="s">
+        <v>224</v>
+      </c>
+      <c r="AU24" t="s">
         <v>62</v>
       </c>
-      <c r="AQ24" t="s">
-        <v>233</v>
-      </c>
-      <c r="AU24" t="s">
-        <v>64</v>
-      </c>
       <c r="AV24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.25">
@@ -3151,10 +3164,10 @@
         <v>61361736950</v>
       </c>
       <c r="F25" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="G25" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="H25" t="s">
         <v>50</v>
@@ -3163,7 +3176,7 @@
         <v>20181028074731</v>
       </c>
       <c r="J25" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="K25">
         <v>176</v>
@@ -3175,46 +3188,46 @@
         <v>53</v>
       </c>
       <c r="O25" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="P25" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="R25" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="S25" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="T25" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="U25">
         <v>593</v>
       </c>
       <c r="V25" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="W25">
         <v>997202510</v>
       </c>
       <c r="Y25" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="AK25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP25" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ25" t="s">
+        <v>224</v>
+      </c>
+      <c r="AU25" t="s">
         <v>62</v>
       </c>
-      <c r="AQ25" t="s">
-        <v>233</v>
-      </c>
-      <c r="AU25" t="s">
-        <v>64</v>
-      </c>
       <c r="AV25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.25">
@@ -3225,76 +3238,76 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E26">
         <v>61362077122</v>
       </c>
       <c r="F26" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="I26">
         <v>20181028111616</v>
       </c>
       <c r="J26" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="K26">
         <v>4398</v>
       </c>
       <c r="L26" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="M26" t="s">
         <v>53</v>
       </c>
       <c r="O26" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="P26" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="R26" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="S26" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="T26" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="U26">
         <v>4002</v>
       </c>
       <c r="V26" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="W26">
         <v>4146026959</v>
       </c>
       <c r="Y26" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="AK26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AM26" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="AN26" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="AP26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ26" t="s">
+        <v>238</v>
+      </c>
+      <c r="AU26" t="s">
         <v>62</v>
       </c>
-      <c r="AQ26" t="s">
-        <v>247</v>
-      </c>
-      <c r="AU26" t="s">
-        <v>64</v>
-      </c>
       <c r="AV26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.25">
@@ -3305,76 +3318,76 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E27">
         <v>61362086393</v>
       </c>
       <c r="F27" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="I27">
         <v>20181028112459</v>
       </c>
       <c r="J27" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="K27">
         <v>5292</v>
       </c>
       <c r="L27" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="M27" t="s">
         <v>53</v>
       </c>
       <c r="O27" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="P27" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="R27" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="S27" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="T27" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="U27">
         <v>4002</v>
       </c>
       <c r="V27" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="W27">
         <v>4146026959</v>
       </c>
       <c r="Y27" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="AK27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AM27" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="AN27" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="AP27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ27" t="s">
+        <v>238</v>
+      </c>
+      <c r="AU27" t="s">
         <v>62</v>
       </c>
-      <c r="AQ27" t="s">
-        <v>247</v>
-      </c>
-      <c r="AU27" t="s">
-        <v>64</v>
-      </c>
       <c r="AV27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.25">
@@ -3385,76 +3398,76 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E28">
         <v>61362093717</v>
       </c>
       <c r="F28" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="I28">
         <v>20181028112940</v>
       </c>
       <c r="J28" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="K28">
         <v>939</v>
       </c>
       <c r="L28" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="M28" t="s">
         <v>53</v>
       </c>
       <c r="O28" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="P28" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="R28" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="S28" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="T28" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="U28">
         <v>4002</v>
       </c>
       <c r="V28" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="W28">
         <v>4146026959</v>
       </c>
       <c r="Y28" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="AK28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AM28" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="AN28" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="AP28" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ28" t="s">
+        <v>238</v>
+      </c>
+      <c r="AU28" t="s">
         <v>62</v>
       </c>
-      <c r="AQ28" t="s">
-        <v>247</v>
-      </c>
-      <c r="AU28" t="s">
-        <v>64</v>
-      </c>
       <c r="AV28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.25">
@@ -3465,76 +3478,76 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E29">
         <v>61362104394</v>
       </c>
       <c r="F29" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="I29">
         <v>20181028113436</v>
       </c>
       <c r="J29" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="K29">
         <v>852</v>
       </c>
       <c r="L29" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="M29" t="s">
         <v>53</v>
       </c>
       <c r="O29" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="P29" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="R29" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="S29" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="T29" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="U29">
         <v>4002</v>
       </c>
       <c r="V29" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="W29">
         <v>4146026959</v>
       </c>
       <c r="Y29" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="AK29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AM29" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="AN29" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="AP29" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ29" t="s">
+        <v>238</v>
+      </c>
+      <c r="AU29" t="s">
         <v>62</v>
       </c>
-      <c r="AQ29" t="s">
-        <v>247</v>
-      </c>
-      <c r="AU29" t="s">
-        <v>64</v>
-      </c>
       <c r="AV29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.25">
@@ -3548,16 +3561,16 @@
         <v>157303</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E30">
         <v>61362343254</v>
       </c>
       <c r="F30" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="G30" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="H30" t="s">
         <v>50</v>
@@ -3566,46 +3579,46 @@
         <v>20181028134246</v>
       </c>
       <c r="J30" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="K30">
         <v>4456.99</v>
       </c>
       <c r="L30" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="M30" t="s">
         <v>53</v>
       </c>
       <c r="O30" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="P30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="R30" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="S30" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="V30" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="AK30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AP30" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ30" t="s">
+        <v>224</v>
+      </c>
+      <c r="AU30" t="s">
         <v>62</v>
       </c>
-      <c r="AQ30" t="s">
-        <v>233</v>
-      </c>
-      <c r="AU30" t="s">
-        <v>64</v>
-      </c>
       <c r="AV30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>